<commit_message>
Update Sim framework version 2 build 2020.03.28.
</commit_message>
<xml_diff>
--- a/2_design/asim/artifacts/testing/analyze-user-item-compare.xlsx
+++ b/2_design/asim/artifacts/testing/analyze-user-item-compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GoogleDrive\todo\working\projects\sim\2_design\asim\artifacts\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958CBF99-0427-4392-A2CF-3F8CF347C3AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6178262C-0D49-4A7B-B9D9-50A399C60BF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{8DB95D20-6883-4AA3-B7D2-5A0EAC39C354}"/>
   </bookViews>
@@ -601,7 +601,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -949,21 +949,37 @@
       <c r="A8" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1">
+        <v>0.78380000000000005</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>0.99409999999999998</v>
+      </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>0.997</v>
+      </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1">
+        <v>0.33850000000000002</v>
+      </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1">
+        <v>3.15E-2</v>
+      </c>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="1">
+        <v>0.8972</v>
+      </c>
       <c r="M8" s="1"/>
-      <c r="N8" s="2"/>
+      <c r="N8" s="2">
+        <v>3.0411000000000001E-2</v>
+      </c>
       <c r="O8" s="2"/>
-      <c r="P8" s="1"/>
+      <c r="P8" s="1">
+        <v>0.23669999999999999</v>
+      </c>
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1203,21 +1219,37 @@
       <c r="A14" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1">
+        <v>0.81320000000000003</v>
+      </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1">
+        <v>1.0622</v>
+      </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1">
+        <v>1.0306</v>
+      </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1">
+        <v>0.2109</v>
+      </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1">
+        <v>2.9100000000000001E-2</v>
+      </c>
       <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="L14" s="1">
+        <v>0.90429999999999999</v>
+      </c>
       <c r="M14" s="1"/>
-      <c r="N14" s="2"/>
+      <c r="N14" s="2">
+        <v>2.8192999999999999E-2</v>
+      </c>
       <c r="O14" s="2"/>
-      <c r="P14" s="1"/>
+      <c r="P14" s="1">
+        <v>0.2641</v>
+      </c>
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1277,21 +1309,37 @@
       <c r="A16" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1">
+        <v>0.78469999999999995</v>
+      </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1">
+        <v>0.99509999999999998</v>
+      </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1">
+        <v>0.99760000000000004</v>
+      </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1">
+        <v>0.23250000000000001</v>
+      </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1">
+        <v>2.24E-2</v>
+      </c>
       <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="L16" s="1">
+        <v>0.45300000000000001</v>
+      </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="2"/>
+      <c r="N16" s="2">
+        <v>2.1333999999999999E-2</v>
+      </c>
       <c r="O16" s="2"/>
-      <c r="P16" s="1"/>
+      <c r="P16" s="1">
+        <v>0.23849999999999999</v>
+      </c>
       <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1504,21 +1552,37 @@
       <c r="A21" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="1">
+        <v>0.77149999999999996</v>
+      </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1">
+        <v>0.97319999999999995</v>
+      </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1">
+        <v>0.98650000000000004</v>
+      </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1">
+        <v>0.35320000000000001</v>
+      </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1">
+        <v>3.2000000000000001E-2</v>
+      </c>
       <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="L21" s="1">
+        <v>0.89980000000000004</v>
+      </c>
       <c r="M21" s="1"/>
-      <c r="N21" s="2"/>
+      <c r="N21" s="2">
+        <v>3.0890999999999998E-2</v>
+      </c>
       <c r="O21" s="2"/>
-      <c r="P21" s="1"/>
+      <c r="P21" s="1">
+        <v>0.23710000000000001</v>
+      </c>
       <c r="Q21" s="1"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -1546,21 +1610,37 @@
       <c r="A23" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1">
+        <v>0.77149999999999996</v>
+      </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1">
+        <v>0.9738</v>
+      </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1">
+        <v>0.98680000000000001</v>
+      </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1">
+        <v>0.35659999999999997</v>
+      </c>
       <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="J23" s="1">
+        <v>3.1800000000000002E-2</v>
+      </c>
       <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="L23" s="1">
+        <v>0.89900000000000002</v>
+      </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="2"/>
+      <c r="N23" s="2">
+        <v>3.0755000000000001E-2</v>
+      </c>
       <c r="O23" s="2"/>
-      <c r="P23" s="1"/>
+      <c r="P23" s="1">
+        <v>0.30680000000000002</v>
+      </c>
       <c r="Q23" s="1"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -2287,21 +2367,37 @@
       <c r="A40" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="1"/>
+      <c r="B40" s="1">
+        <v>0.78249999999999997</v>
+      </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
+      <c r="D40" s="1">
+        <v>0.9909</v>
+      </c>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="F40" s="1">
+        <v>0.99550000000000005</v>
+      </c>
       <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="H40" s="1">
+        <v>0.3422</v>
+      </c>
       <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="J40" s="1">
+        <v>3.1600000000000003E-2</v>
+      </c>
       <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
+      <c r="L40" s="1">
+        <v>0.89710000000000001</v>
+      </c>
       <c r="M40" s="1"/>
-      <c r="N40" s="2"/>
+      <c r="N40" s="2">
+        <v>3.0483E-2</v>
+      </c>
       <c r="O40" s="2"/>
-      <c r="P40" s="1"/>
+      <c r="P40" s="1">
+        <v>0.34489999999999998</v>
+      </c>
       <c r="Q40" s="1"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>